<commit_message>
Updated Menu and Messages to use new SDL and got them all working... or as far as I think. They both display as they're suppose to. Haven't tested adding messages but first message adds correctly so...
</commit_message>
<xml_diff>
--- a/Development Docs/ADV_Magic_ouline.xlsx
+++ b/Development Docs/ADV_Magic_ouline.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="7740" tabRatio="667"/>
@@ -15,12 +15,12 @@
     <sheet name="Damage Tests" sheetId="6" r:id="rId6"/>
     <sheet name="Weapon List" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="447">
   <si>
     <t>Holy</t>
   </si>
@@ -1339,9 +1339,6 @@
     <t>gravity?</t>
   </si>
   <si>
-    <t>immobilize</t>
-  </si>
-  <si>
     <t>invisible</t>
   </si>
   <si>
@@ -1355,17 +1352,26 @@
   </si>
   <si>
     <t>how about damage plus status effect</t>
+  </si>
+  <si>
+    <t>paralize</t>
+  </si>
+  <si>
+    <t>MP poison</t>
+  </si>
+  <si>
+    <t>EVA raise.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1562,10 +1568,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1579,6 +1585,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1657,6 +1668,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1691,6 +1703,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1866,14 +1879,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
@@ -1883,7 +1896,7 @@
     <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1913,12 +1926,12 @@
       </c>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100</v>
       </c>
@@ -1933,8 +1946,11 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="K5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>75</v>
       </c>
@@ -1953,7 +1969,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50</v>
       </c>
@@ -1982,7 +1998,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25</v>
       </c>
@@ -2010,8 +2026,11 @@
       <c r="I8" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="K8" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -2033,7 +2052,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2062,15 +2081,15 @@
         <v>12</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K11" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>436</v>
       </c>
@@ -2080,30 +2099,30 @@
       <c r="E12" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" t="s">
+        <v>444</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="K12" t="s">
         <v>439</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>442</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="K12" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2117,7 +2136,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>48</v>
       </c>
@@ -2125,7 +2144,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -2149,7 +2168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>43</v>
       </c>
@@ -2173,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>37</v>
       </c>
@@ -2197,7 +2216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2209,7 +2228,7 @@
         <v>53.125</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -2224,7 +2243,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E27" s="3" t="s">
         <v>46</v>
       </c>
@@ -2233,47 +2252,47 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>151</v>
       </c>
@@ -2281,7 +2300,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1">
+    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>147</v>
       </c>
@@ -2292,10 +2311,10 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="72" customHeight="1" thickBot="1">
+    <row r="42" spans="1:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
@@ -2306,27 +2325,27 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>158</v>
       </c>
@@ -2338,14 +2357,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
@@ -2362,17 +2381,17 @@
     <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -2380,7 +2399,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2388,7 +2407,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -2396,7 +2415,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -2404,7 +2423,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -2412,7 +2431,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -2420,17 +2439,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -2438,7 +2457,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -2446,7 +2465,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -2454,7 +2473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -2462,7 +2481,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -2470,17 +2489,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N21" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N22" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>175</v>
       </c>
@@ -2497,7 +2516,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>176</v>
       </c>
@@ -2526,7 +2545,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>177</v>
       </c>
@@ -2570,7 +2589,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>178</v>
       </c>
@@ -2614,7 +2633,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2658,7 +2677,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -2690,7 +2709,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -2701,7 +2720,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -2712,7 +2731,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -2732,7 +2751,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -2752,7 +2771,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L33" t="s">
         <v>221</v>
       </c>
@@ -2760,7 +2779,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>188</v>
       </c>
@@ -2775,24 +2794,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>240</v>
       </c>
@@ -2803,7 +2822,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -2820,7 +2839,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -2843,7 +2862,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -2866,7 +2885,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -2889,7 +2908,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -2912,7 +2931,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -2935,7 +2954,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L10" t="s">
         <v>99</v>
       </c>
@@ -2949,7 +2968,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -2969,7 +2988,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>88</v>
       </c>
@@ -2983,7 +3002,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -2997,7 +3016,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -3011,7 +3030,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L15" t="s">
         <v>111</v>
       </c>
@@ -3019,7 +3038,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -3033,7 +3052,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -3041,7 +3060,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -3049,7 +3068,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>118</v>
       </c>
@@ -3060,7 +3079,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -3071,7 +3090,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>120</v>
       </c>
@@ -3079,7 +3098,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -3087,7 +3106,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>129</v>
       </c>
@@ -3095,7 +3114,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -3103,7 +3122,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>160</v>
       </c>
@@ -3117,30 +3136,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>238</v>
       </c>
@@ -3154,7 +3173,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3166,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3179,7 +3198,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3192,7 +3211,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -3205,7 +3224,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -3218,7 +3237,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -3231,7 +3250,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -3244,7 +3263,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -3257,7 +3276,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -3270,7 +3289,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -3283,7 +3302,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -3296,7 +3315,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -3309,7 +3328,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -3322,7 +3341,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -3335,7 +3354,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -3348,7 +3367,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -3361,7 +3380,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -3374,7 +3393,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -3387,7 +3406,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -3400,7 +3419,7 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -3413,7 +3432,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -3426,7 +3445,7 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -3439,7 +3458,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -3452,7 +3471,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -3465,7 +3484,7 @@
         <v>4700</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -3478,7 +3497,7 @@
         <v>4900</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -3491,7 +3510,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -3504,7 +3523,7 @@
         <v>5300</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -3517,7 +3536,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -3530,7 +3549,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -3543,7 +3562,7 @@
         <v>5900</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -3556,7 +3575,7 @@
         <v>6100</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -3569,7 +3588,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -3582,7 +3601,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -3595,7 +3614,7 @@
         <v>6700</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -3608,7 +3627,7 @@
         <v>6900</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
@@ -3621,7 +3640,7 @@
         <v>7100</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -3634,7 +3653,7 @@
         <v>7300</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -3647,7 +3666,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -3660,7 +3679,7 @@
         <v>7700</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -3673,7 +3692,7 @@
         <v>7900</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
@@ -3686,7 +3705,7 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
@@ -3699,7 +3718,7 @@
         <v>8300</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
@@ -3712,7 +3731,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
@@ -3725,7 +3744,7 @@
         <v>8700</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
@@ -3738,7 +3757,7 @@
         <v>8900</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
@@ -3751,7 +3770,7 @@
         <v>9100</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
@@ -3764,7 +3783,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
@@ -3777,7 +3796,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
@@ -3790,7 +3809,7 @@
         <v>9700</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -3803,7 +3822,7 @@
         <v>9900</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
@@ -3816,7 +3835,7 @@
         <v>10100</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
@@ -3829,7 +3848,7 @@
         <v>10300</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
@@ -3842,7 +3861,7 @@
         <v>10500</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
@@ -3855,7 +3874,7 @@
         <v>10700</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
@@ -3868,7 +3887,7 @@
         <v>10900</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
@@ -3881,7 +3900,7 @@
         <v>11100</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
@@ -3894,7 +3913,7 @@
         <v>11300</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
@@ -3907,7 +3926,7 @@
         <v>11500</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
@@ -3920,7 +3939,7 @@
         <v>11700</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>
@@ -3933,7 +3952,7 @@
         <v>11900</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>61</v>
       </c>
@@ -3946,7 +3965,7 @@
         <v>12100</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>62</v>
       </c>
@@ -3959,7 +3978,7 @@
         <v>12300</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>63</v>
       </c>
@@ -3972,7 +3991,7 @@
         <v>12500</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>64</v>
       </c>
@@ -3985,7 +4004,7 @@
         <v>12700</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>65</v>
       </c>
@@ -3998,7 +4017,7 @@
         <v>12900</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>66</v>
       </c>
@@ -4011,7 +4030,7 @@
         <v>13100</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>67</v>
       </c>
@@ -4024,7 +4043,7 @@
         <v>13300</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>68</v>
       </c>
@@ -4037,7 +4056,7 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>69</v>
       </c>
@@ -4050,7 +4069,7 @@
         <v>13700</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>70</v>
       </c>
@@ -4063,7 +4082,7 @@
         <v>13900</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>71</v>
       </c>
@@ -4076,7 +4095,7 @@
         <v>14100</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>72</v>
       </c>
@@ -4089,7 +4108,7 @@
         <v>14300</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>73</v>
       </c>
@@ -4102,7 +4121,7 @@
         <v>14500</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>74</v>
       </c>
@@ -4115,7 +4134,7 @@
         <v>14700</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>75</v>
       </c>
@@ -4128,7 +4147,7 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>76</v>
       </c>
@@ -4141,7 +4160,7 @@
         <v>15100</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>77</v>
       </c>
@@ -4154,7 +4173,7 @@
         <v>15300</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>78</v>
       </c>
@@ -4167,7 +4186,7 @@
         <v>15500</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>79</v>
       </c>
@@ -4180,7 +4199,7 @@
         <v>15700</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>80</v>
       </c>
@@ -4193,7 +4212,7 @@
         <v>15900</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>81</v>
       </c>
@@ -4206,7 +4225,7 @@
         <v>16100</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>82</v>
       </c>
@@ -4219,7 +4238,7 @@
         <v>16300</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>83</v>
       </c>
@@ -4232,7 +4251,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>84</v>
       </c>
@@ -4245,7 +4264,7 @@
         <v>16700</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>85</v>
       </c>
@@ -4258,7 +4277,7 @@
         <v>16900</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>86</v>
       </c>
@@ -4271,7 +4290,7 @@
         <v>17100</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>87</v>
       </c>
@@ -4284,7 +4303,7 @@
         <v>17300</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>88</v>
       </c>
@@ -4297,7 +4316,7 @@
         <v>17500</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>89</v>
       </c>
@@ -4310,7 +4329,7 @@
         <v>17700</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>90</v>
       </c>
@@ -4323,7 +4342,7 @@
         <v>17900</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>91</v>
       </c>
@@ -4336,7 +4355,7 @@
         <v>18100</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>92</v>
       </c>
@@ -4349,7 +4368,7 @@
         <v>18300</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>93</v>
       </c>
@@ -4362,7 +4381,7 @@
         <v>18500</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>94</v>
       </c>
@@ -4375,7 +4394,7 @@
         <v>18700</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>95</v>
       </c>
@@ -4388,7 +4407,7 @@
         <v>18900</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>96</v>
       </c>
@@ -4401,7 +4420,7 @@
         <v>19100</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>97</v>
       </c>
@@ -4414,7 +4433,7 @@
         <v>19300</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>98</v>
       </c>
@@ -4427,7 +4446,7 @@
         <v>19500</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>99</v>
       </c>
@@ -4440,7 +4459,7 @@
         <v>19700</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>100</v>
       </c>
@@ -4453,7 +4472,7 @@
         <v>19900</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>101</v>
       </c>
@@ -4466,7 +4485,7 @@
         <v>20100</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>102</v>
       </c>
@@ -4479,7 +4498,7 @@
         <v>20300</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>103</v>
       </c>
@@ -4492,7 +4511,7 @@
         <v>20500</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>104</v>
       </c>
@@ -4505,7 +4524,7 @@
         <v>20700</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>105</v>
       </c>
@@ -4518,7 +4537,7 @@
         <v>20900</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>106</v>
       </c>
@@ -4531,7 +4550,7 @@
         <v>21100</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>107</v>
       </c>
@@ -4544,7 +4563,7 @@
         <v>21300</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>108</v>
       </c>
@@ -4557,7 +4576,7 @@
         <v>21500</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>109</v>
       </c>
@@ -4570,7 +4589,7 @@
         <v>21700</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>110</v>
       </c>
@@ -4583,7 +4602,7 @@
         <v>21900</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>111</v>
       </c>
@@ -4596,7 +4615,7 @@
         <v>22100</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>112</v>
       </c>
@@ -4609,7 +4628,7 @@
         <v>22300</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>113</v>
       </c>
@@ -4622,7 +4641,7 @@
         <v>22500</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>114</v>
       </c>
@@ -4635,7 +4654,7 @@
         <v>22700</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>115</v>
       </c>
@@ -4648,7 +4667,7 @@
         <v>22900</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>116</v>
       </c>
@@ -4661,7 +4680,7 @@
         <v>23100</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>117</v>
       </c>
@@ -4674,7 +4693,7 @@
         <v>23300</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>118</v>
       </c>
@@ -4687,7 +4706,7 @@
         <v>23500</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>119</v>
       </c>
@@ -4700,7 +4719,7 @@
         <v>23700</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>120</v>
       </c>
@@ -4713,7 +4732,7 @@
         <v>23900</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>121</v>
       </c>
@@ -4726,7 +4745,7 @@
         <v>24100</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>122</v>
       </c>
@@ -4739,7 +4758,7 @@
         <v>24300</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>123</v>
       </c>
@@ -4752,7 +4771,7 @@
         <v>24500</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>124</v>
       </c>
@@ -4765,7 +4784,7 @@
         <v>24700</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>125</v>
       </c>
@@ -4778,7 +4797,7 @@
         <v>24900</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>126</v>
       </c>
@@ -4791,7 +4810,7 @@
         <v>25100</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>127</v>
       </c>
@@ -4804,7 +4823,7 @@
         <v>25300</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>128</v>
       </c>
@@ -4817,7 +4836,7 @@
         <v>25500</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>129</v>
       </c>
@@ -4830,7 +4849,7 @@
         <v>25700</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>130</v>
       </c>
@@ -4843,7 +4862,7 @@
         <v>25900</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>131</v>
       </c>
@@ -4856,7 +4875,7 @@
         <v>26100</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>132</v>
       </c>
@@ -4869,7 +4888,7 @@
         <v>26300</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>133</v>
       </c>
@@ -4882,7 +4901,7 @@
         <v>26500</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>134</v>
       </c>
@@ -4895,7 +4914,7 @@
         <v>26700</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>135</v>
       </c>
@@ -4908,7 +4927,7 @@
         <v>26900</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>136</v>
       </c>
@@ -4921,7 +4940,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>137</v>
       </c>
@@ -4934,7 +4953,7 @@
         <v>27300</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>138</v>
       </c>
@@ -4947,7 +4966,7 @@
         <v>27500</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>139</v>
       </c>
@@ -4960,7 +4979,7 @@
         <v>27700</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>140</v>
       </c>
@@ -4973,7 +4992,7 @@
         <v>27900</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>141</v>
       </c>
@@ -4986,7 +5005,7 @@
         <v>28100</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>142</v>
       </c>
@@ -4999,7 +5018,7 @@
         <v>28300</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>143</v>
       </c>
@@ -5012,7 +5031,7 @@
         <v>28500</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>144</v>
       </c>
@@ -5025,7 +5044,7 @@
         <v>28700</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>145</v>
       </c>
@@ -5038,7 +5057,7 @@
         <v>28900</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>146</v>
       </c>
@@ -5051,7 +5070,7 @@
         <v>29100</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>147</v>
       </c>
@@ -5064,7 +5083,7 @@
         <v>29300</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>148</v>
       </c>
@@ -5077,7 +5096,7 @@
         <v>29500</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>149</v>
       </c>
@@ -5090,7 +5109,7 @@
         <v>29700</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>150</v>
       </c>
@@ -5103,7 +5122,7 @@
         <v>29900</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>151</v>
       </c>
@@ -5116,7 +5135,7 @@
         <v>30100</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>152</v>
       </c>
@@ -5129,7 +5148,7 @@
         <v>30300</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>153</v>
       </c>
@@ -5142,7 +5161,7 @@
         <v>30500</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>154</v>
       </c>
@@ -5155,7 +5174,7 @@
         <v>30700</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>155</v>
       </c>
@@ -5168,7 +5187,7 @@
         <v>30900</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>156</v>
       </c>
@@ -5181,7 +5200,7 @@
         <v>31100</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>157</v>
       </c>
@@ -5194,7 +5213,7 @@
         <v>31300</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>158</v>
       </c>
@@ -5207,7 +5226,7 @@
         <v>31500</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>159</v>
       </c>
@@ -5220,7 +5239,7 @@
         <v>31700</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>160</v>
       </c>
@@ -5233,7 +5252,7 @@
         <v>31900</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>161</v>
       </c>
@@ -5246,7 +5265,7 @@
         <v>32100</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>162</v>
       </c>
@@ -5259,7 +5278,7 @@
         <v>32300</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>163</v>
       </c>
@@ -5272,7 +5291,7 @@
         <v>32500</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>164</v>
       </c>
@@ -5285,7 +5304,7 @@
         <v>32700</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>165</v>
       </c>
@@ -5298,7 +5317,7 @@
         <v>32900</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>166</v>
       </c>
@@ -5311,7 +5330,7 @@
         <v>33100</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>167</v>
       </c>
@@ -5324,7 +5343,7 @@
         <v>33300</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>168</v>
       </c>
@@ -5337,7 +5356,7 @@
         <v>33500</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>169</v>
       </c>
@@ -5350,7 +5369,7 @@
         <v>33700</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>170</v>
       </c>
@@ -5363,7 +5382,7 @@
         <v>33900</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>171</v>
       </c>
@@ -5376,7 +5395,7 @@
         <v>34100</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>172</v>
       </c>
@@ -5389,7 +5408,7 @@
         <v>34300</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>173</v>
       </c>
@@ -5402,7 +5421,7 @@
         <v>34500</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>174</v>
       </c>
@@ -5415,7 +5434,7 @@
         <v>34700</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>175</v>
       </c>
@@ -5428,7 +5447,7 @@
         <v>34900</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>176</v>
       </c>
@@ -5441,7 +5460,7 @@
         <v>35100</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>177</v>
       </c>
@@ -5454,7 +5473,7 @@
         <v>35300</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>178</v>
       </c>
@@ -5467,7 +5486,7 @@
         <v>35500</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>179</v>
       </c>
@@ -5480,7 +5499,7 @@
         <v>35700</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>180</v>
       </c>
@@ -5493,7 +5512,7 @@
         <v>35900</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>181</v>
       </c>
@@ -5506,7 +5525,7 @@
         <v>36100</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>182</v>
       </c>
@@ -5519,7 +5538,7 @@
         <v>36300</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>183</v>
       </c>
@@ -5532,7 +5551,7 @@
         <v>36500</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>184</v>
       </c>
@@ -5545,7 +5564,7 @@
         <v>36700</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>185</v>
       </c>
@@ -5558,7 +5577,7 @@
         <v>36900</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>186</v>
       </c>
@@ -5571,7 +5590,7 @@
         <v>37100</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>187</v>
       </c>
@@ -5584,7 +5603,7 @@
         <v>37300</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>188</v>
       </c>
@@ -5597,7 +5616,7 @@
         <v>37500</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>189</v>
       </c>
@@ -5610,7 +5629,7 @@
         <v>37700</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>190</v>
       </c>
@@ -5623,7 +5642,7 @@
         <v>37900</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>191</v>
       </c>
@@ -5636,7 +5655,7 @@
         <v>38100</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>192</v>
       </c>
@@ -5649,7 +5668,7 @@
         <v>38300</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>193</v>
       </c>
@@ -5662,7 +5681,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>194</v>
       </c>
@@ -5675,7 +5694,7 @@
         <v>38700</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>195</v>
       </c>
@@ -5688,7 +5707,7 @@
         <v>38900</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>196</v>
       </c>
@@ -5701,7 +5720,7 @@
         <v>39100</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>197</v>
       </c>
@@ -5714,7 +5733,7 @@
         <v>39300</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>198</v>
       </c>
@@ -5727,7 +5746,7 @@
         <v>39500</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>199</v>
       </c>
@@ -5740,7 +5759,7 @@
         <v>39700</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>200</v>
       </c>
@@ -5753,7 +5772,7 @@
         <v>39900</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>201</v>
       </c>
@@ -5766,7 +5785,7 @@
         <v>40100</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>202</v>
       </c>
@@ -5779,7 +5798,7 @@
         <v>40300</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>203</v>
       </c>
@@ -5792,7 +5811,7 @@
         <v>40500</v>
       </c>
     </row>
-    <row r="207" spans="1:3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>204</v>
       </c>
@@ -5805,7 +5824,7 @@
         <v>40700</v>
       </c>
     </row>
-    <row r="208" spans="1:3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>205</v>
       </c>
@@ -5818,7 +5837,7 @@
         <v>40900</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>206</v>
       </c>
@@ -5831,7 +5850,7 @@
         <v>41100</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>207</v>
       </c>
@@ -5844,7 +5863,7 @@
         <v>41300</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>208</v>
       </c>
@@ -5857,7 +5876,7 @@
         <v>41500</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>209</v>
       </c>
@@ -5870,7 +5889,7 @@
         <v>41700</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>210</v>
       </c>
@@ -5883,7 +5902,7 @@
         <v>41900</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>211</v>
       </c>
@@ -5896,7 +5915,7 @@
         <v>42100</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>212</v>
       </c>
@@ -5909,7 +5928,7 @@
         <v>42300</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>213</v>
       </c>
@@ -5922,7 +5941,7 @@
         <v>42500</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>214</v>
       </c>
@@ -5935,7 +5954,7 @@
         <v>42700</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>215</v>
       </c>
@@ -5948,7 +5967,7 @@
         <v>42900</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>216</v>
       </c>
@@ -5961,7 +5980,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>217</v>
       </c>
@@ -5974,7 +5993,7 @@
         <v>43300</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>218</v>
       </c>
@@ -5987,7 +6006,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>219</v>
       </c>
@@ -6000,7 +6019,7 @@
         <v>43700</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>220</v>
       </c>
@@ -6013,7 +6032,7 @@
         <v>43900</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>221</v>
       </c>
@@ -6026,7 +6045,7 @@
         <v>44100</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>222</v>
       </c>
@@ -6039,7 +6058,7 @@
         <v>44300</v>
       </c>
     </row>
-    <row r="226" spans="1:3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>223</v>
       </c>
@@ -6052,7 +6071,7 @@
         <v>44500</v>
       </c>
     </row>
-    <row r="227" spans="1:3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>224</v>
       </c>
@@ -6065,7 +6084,7 @@
         <v>44700</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>225</v>
       </c>
@@ -6078,7 +6097,7 @@
         <v>44900</v>
       </c>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>226</v>
       </c>
@@ -6091,7 +6110,7 @@
         <v>45100</v>
       </c>
     </row>
-    <row r="230" spans="1:3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>227</v>
       </c>
@@ -6104,7 +6123,7 @@
         <v>45300</v>
       </c>
     </row>
-    <row r="231" spans="1:3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>228</v>
       </c>
@@ -6117,7 +6136,7 @@
         <v>45500</v>
       </c>
     </row>
-    <row r="232" spans="1:3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>229</v>
       </c>
@@ -6130,7 +6149,7 @@
         <v>45700</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>230</v>
       </c>
@@ -6143,7 +6162,7 @@
         <v>45900</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>231</v>
       </c>
@@ -6156,7 +6175,7 @@
         <v>46100</v>
       </c>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>232</v>
       </c>
@@ -6169,7 +6188,7 @@
         <v>46300</v>
       </c>
     </row>
-    <row r="236" spans="1:3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>233</v>
       </c>
@@ -6182,7 +6201,7 @@
         <v>46500</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>234</v>
       </c>
@@ -6195,7 +6214,7 @@
         <v>46700</v>
       </c>
     </row>
-    <row r="238" spans="1:3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>235</v>
       </c>
@@ -6208,7 +6227,7 @@
         <v>46900</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>236</v>
       </c>
@@ -6221,7 +6240,7 @@
         <v>47100</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>237</v>
       </c>
@@ -6234,7 +6253,7 @@
         <v>47300</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>238</v>
       </c>
@@ -6247,7 +6266,7 @@
         <v>47500</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>239</v>
       </c>
@@ -6260,7 +6279,7 @@
         <v>47700</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>240</v>
       </c>
@@ -6273,7 +6292,7 @@
         <v>47900</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>241</v>
       </c>
@@ -6286,7 +6305,7 @@
         <v>48100</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>242</v>
       </c>
@@ -6299,7 +6318,7 @@
         <v>48300</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>243</v>
       </c>
@@ -6312,7 +6331,7 @@
         <v>48500</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>244</v>
       </c>
@@ -6325,7 +6344,7 @@
         <v>48700</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>245</v>
       </c>
@@ -6338,7 +6357,7 @@
         <v>48900</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>246</v>
       </c>
@@ -6351,7 +6370,7 @@
         <v>49100</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>247</v>
       </c>
@@ -6364,7 +6383,7 @@
         <v>49300</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>248</v>
       </c>
@@ -6377,7 +6396,7 @@
         <v>49500</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>249</v>
       </c>
@@ -6390,7 +6409,7 @@
         <v>49700</v>
       </c>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>250</v>
       </c>
@@ -6403,7 +6422,7 @@
         <v>49900</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>251</v>
       </c>
@@ -6416,7 +6435,7 @@
         <v>50100</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>252</v>
       </c>
@@ -6429,7 +6448,7 @@
         <v>50300</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>253</v>
       </c>
@@ -6442,7 +6461,7 @@
         <v>50500</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>254</v>
       </c>
@@ -6455,7 +6474,7 @@
         <v>50700</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>255</v>
       </c>
@@ -6474,14 +6493,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -6496,12 +6515,12 @@
     <col min="12" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.25">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>255</v>
       </c>
@@ -6527,7 +6546,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>277</v>
       </c>
@@ -6540,7 +6559,7 @@
       <c r="D4" t="s">
         <v>317</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>328</v>
       </c>
       <c r="F4" t="s">
@@ -6553,16 +6572,16 @@
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
-      <c r="E5" s="31"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E5" s="30"/>
       <c r="G5" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="E6" s="31"/>
-    </row>
-    <row r="7" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E6" s="30"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>278</v>
       </c>
@@ -6588,16 +6607,16 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E8" s="29"/>
       <c r="G8" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E9" s="29"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>280</v>
       </c>
@@ -6623,7 +6642,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E11" s="29"/>
       <c r="F11" t="s">
         <v>343</v>
@@ -6632,10 +6651,10 @@
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E12" s="29"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -6661,16 +6680,16 @@
         <v>281</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E14" s="29"/>
       <c r="G14" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E15" s="29"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -6683,7 +6702,7 @@
       <c r="D16" t="s">
         <v>317</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="31" t="s">
         <v>334</v>
       </c>
       <c r="F16" t="s">
@@ -6696,16 +6715,16 @@
         <v>285</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
-      <c r="E17" s="30"/>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E17" s="31"/>
       <c r="G17" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
-      <c r="E18" s="30"/>
-    </row>
-    <row r="19" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E18" s="31"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -6731,7 +6750,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -6741,10 +6760,10 @@
         <v>275</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E21" s="29"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>288</v>
       </c>
@@ -6770,16 +6789,16 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E23" s="29"/>
       <c r="G23" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E24" s="29"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>290</v>
       </c>
@@ -6805,7 +6824,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E26" s="29"/>
       <c r="F26" t="s">
         <v>340</v>
@@ -6814,10 +6833,10 @@
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E27" s="29"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>293</v>
       </c>
@@ -6830,7 +6849,7 @@
       <c r="D28" t="s">
         <v>322</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="31" t="s">
         <v>341</v>
       </c>
       <c r="F28" t="s">
@@ -6843,8 +6862,8 @@
         <v>294</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
-      <c r="E29" s="30"/>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E29" s="31"/>
       <c r="F29" t="s">
         <v>340</v>
       </c>
@@ -6852,10 +6871,10 @@
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
-      <c r="E30" s="30"/>
-    </row>
-    <row r="31" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E30" s="31"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>296</v>
       </c>
@@ -6868,7 +6887,7 @@
       <c r="D31" t="s">
         <v>317</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="31" t="s">
         <v>344</v>
       </c>
       <c r="F31" t="s">
@@ -6881,16 +6900,16 @@
         <v>294</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
-      <c r="E32" s="30"/>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E32" s="31"/>
       <c r="G32" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
-      <c r="E33" s="30"/>
-    </row>
-    <row r="34" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E33" s="31"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>298</v>
       </c>
@@ -6903,7 +6922,7 @@
       <c r="D34" t="s">
         <v>317</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="E34" s="31" t="s">
         <v>345</v>
       </c>
       <c r="F34" t="s">
@@ -6916,16 +6935,16 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
-      <c r="E35" s="30"/>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E35" s="31"/>
       <c r="G35" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
-      <c r="E36" s="30"/>
-    </row>
-    <row r="37" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E36" s="31"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>300</v>
       </c>
@@ -6938,7 +6957,7 @@
       <c r="D37" t="s">
         <v>317</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="E37" s="31" t="s">
         <v>347</v>
       </c>
       <c r="F37" t="s">
@@ -6951,16 +6970,16 @@
         <v>294</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
-      <c r="E38" s="30"/>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E38" s="31"/>
       <c r="G38" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
-      <c r="E39" s="30"/>
-    </row>
-    <row r="40" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E39" s="31"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>302</v>
       </c>
@@ -6986,7 +7005,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E41" s="29"/>
       <c r="F41" t="s">
         <v>332</v>
@@ -6995,10 +7014,10 @@
         <v>292</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E42" s="29"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>304</v>
       </c>
@@ -7024,7 +7043,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E44" s="29"/>
       <c r="F44" t="s">
         <v>342</v>
@@ -7033,13 +7052,13 @@
         <v>292</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E45" s="29"/>
       <c r="F45" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>306</v>
       </c>
@@ -7065,7 +7084,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E47" s="29"/>
       <c r="F47" t="s">
         <v>351</v>
@@ -7074,10 +7093,10 @@
         <v>275</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E48" s="29"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>309</v>
       </c>
@@ -7090,7 +7109,7 @@
       <c r="D49" t="s">
         <v>317</v>
       </c>
-      <c r="E49" s="30" t="s">
+      <c r="E49" s="31" t="s">
         <v>352</v>
       </c>
       <c r="F49" t="s">
@@ -7103,8 +7122,8 @@
         <v>305</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
-      <c r="E50" s="30"/>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E50" s="31"/>
       <c r="F50" t="s">
         <v>342</v>
       </c>
@@ -7112,42 +7131,36 @@
         <v>275</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
-      <c r="E51" s="30"/>
-    </row>
-    <row r="54" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E51" s="31"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>357</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="E16:E18"/>
     <mergeCell ref="E40:E42"/>
     <mergeCell ref="E43:E45"/>
     <mergeCell ref="E46:E48"/>
@@ -7158,20 +7171,26 @@
     <mergeCell ref="E31:E33"/>
     <mergeCell ref="E34:E36"/>
     <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="E16:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
@@ -7185,23 +7204,23 @@
     <col min="10" max="10" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="8" spans="1:10">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" s="32" t="s">
         <v>261</v>
       </c>
@@ -7219,7 +7238,7 @@
       </c>
       <c r="J8" s="33"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>259</v>
       </c>
@@ -7250,7 +7269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>55</v>
       </c>
@@ -7281,7 +7300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>260</v>
       </c>
@@ -7312,7 +7331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>268</v>
       </c>
@@ -7341,7 +7360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
       <c r="E13" s="10"/>
@@ -7351,7 +7370,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>263</v>
       </c>
@@ -7364,7 +7383,7 @@
       <c r="I14" s="10"/>
       <c r="J14" s="11"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>269</v>
       </c>
@@ -7377,7 +7396,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="10"/>
@@ -7387,7 +7406,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>265</v>
       </c>
@@ -7412,7 +7431,7 @@
       </c>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>266</v>
       </c>
@@ -7437,7 +7456,7 @@
       </c>
       <c r="J18" s="11"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
       <c r="D19" s="11"/>
       <c r="E19" s="10"/>
@@ -7447,7 +7466,7 @@
       <c r="I19" s="10"/>
       <c r="J19" s="11"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>267</v>
       </c>
@@ -7472,7 +7491,7 @@
       </c>
       <c r="J20" s="11"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
       <c r="E21" s="10"/>
@@ -7482,7 +7501,7 @@
       <c r="I21" s="10"/>
       <c r="J21" s="11"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="10"/>
@@ -7492,7 +7511,7 @@
       <c r="I22" s="10"/>
       <c r="J22" s="11"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>270</v>
       </c>
@@ -7517,7 +7536,7 @@
       </c>
       <c r="J23" s="11"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>267</v>
       </c>
@@ -7542,7 +7561,7 @@
       </c>
       <c r="J24" s="11"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C25" s="10"/>
       <c r="D25" s="11"/>
       <c r="E25" s="10"/>
@@ -7552,7 +7571,7 @@
       <c r="I25" s="10"/>
       <c r="J25" s="11"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>276</v>
       </c>
@@ -7582,7 +7601,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="15">
@@ -7630,7 +7649,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1">
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="17">
@@ -7678,13 +7697,13 @@
         <v>46.09375</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>277</v>
       </c>
@@ -7695,12 +7714,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>278</v>
       </c>
@@ -7711,12 +7730,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>280</v>
       </c>
@@ -7724,7 +7743,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>110</v>
       </c>
@@ -7738,12 +7757,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -7757,12 +7776,12 @@
         <v>285</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -7776,7 +7795,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>287</v>
       </c>
@@ -7784,7 +7803,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>288</v>
       </c>
@@ -7798,12 +7817,12 @@
         <v>285</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>290</v>
       </c>
@@ -7817,12 +7836,12 @@
         <v>285</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>293</v>
       </c>
@@ -7839,12 +7858,12 @@
         <v>297</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>296</v>
       </c>
@@ -7858,12 +7877,12 @@
         <v>295</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>298</v>
       </c>
@@ -7877,12 +7896,12 @@
         <v>299</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>300</v>
       </c>
@@ -7896,12 +7915,12 @@
         <v>301</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>302</v>
       </c>
@@ -7915,12 +7934,12 @@
         <v>303</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>304</v>
       </c>
@@ -7934,12 +7953,12 @@
         <v>305</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>306</v>
       </c>
@@ -7953,12 +7972,12 @@
         <v>308</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>309</v>
       </c>
@@ -7972,7 +7991,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>275</v>
       </c>
@@ -7990,396 +8009,396 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A85"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>423</v>
       </c>

</xml_diff>

<commit_message>
Actions Now work and Updated VG Planning doc which is the design doc... needs to be renamed.
</commit_message>
<xml_diff>
--- a/Development Docs/ADV_Magic_ouline.xlsx
+++ b/Development Docs/ADV_Magic_ouline.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="479">
   <si>
     <t>Holy</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Basic Type</t>
   </si>
   <si>
-    <t>Thunder</t>
-  </si>
-  <si>
     <t>Earth</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Blind</t>
   </si>
   <si>
-    <t>Poison</t>
-  </si>
-  <si>
     <t>Sleep</t>
   </si>
   <si>
@@ -109,12 +103,6 @@
     <t>Magic Reflect</t>
   </si>
   <si>
-    <t>SkillBuff</t>
-  </si>
-  <si>
-    <t>Drain is like poison, which constantly reduces your HP, but also gives them to the person who inflicted you with drain</t>
-  </si>
-  <si>
     <t>MP Blast</t>
   </si>
   <si>
@@ -175,9 +163,6 @@
     <t>Lowers cost by 2%</t>
   </si>
   <si>
-    <t>Raises power by 25%%</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -454,9 +439,6 @@
     <t>It’s an awesome idea but it then only incorporates two of the modifiers</t>
   </si>
   <si>
-    <t>Wht if we have multiple slider bars… One for Power/Efficiency,  one for AOE/Speed</t>
-  </si>
-  <si>
     <t>what if it was a slider triangle… or a slider box… then each point you put in the box would be 1/4 of a bar</t>
   </si>
   <si>
@@ -481,9 +463,6 @@
     <t>increases Area of Effect</t>
   </si>
   <si>
-    <t>but then it is always either always have to be square, or its going to end up being a fucked up polygon</t>
-  </si>
-  <si>
     <t>Also this presents a problem, because it still doesn't answer the efficiency problem, how does the efficiency portion of the equasion, does raising power raise the cost?</t>
   </si>
   <si>
@@ -640,9 +619,6 @@
     <t>STR, Profficiencies</t>
   </si>
   <si>
-    <t>HP, Vitality, Magic Defense</t>
-  </si>
-  <si>
     <t>MP, or AP</t>
   </si>
   <si>
@@ -1072,9 +1048,6 @@
     <t>Hand Crafted Throwing Bombs, with a variety of different effects. The Range and accuracy is dependent on the User's Strength and Dexterity.</t>
   </si>
   <si>
-    <t>A long pole with a blade or point on the end. The User gaints a range advantage but sacrifices his ability to equip a shield.</t>
-  </si>
-  <si>
     <t>DEX - Low</t>
   </si>
   <si>
@@ -1327,21 +1300,12 @@
     <t>Att Buff</t>
   </si>
   <si>
-    <t>Sap Drain</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
     <t>stop</t>
   </si>
   <si>
     <t>gravity?</t>
   </si>
   <si>
-    <t>invisible</t>
-  </si>
-  <si>
     <t>insta death</t>
   </si>
   <si>
@@ -1357,10 +1321,142 @@
     <t>paralize</t>
   </si>
   <si>
-    <t>MP poison</t>
-  </si>
-  <si>
     <t>EVA raise.</t>
+  </si>
+  <si>
+    <t>HP, Vitality, Magic Defense, Spirit</t>
+  </si>
+  <si>
+    <t>What if we have multiple slider bars… One for Power/Efficiency,  one for AOE/Speed</t>
+  </si>
+  <si>
+    <t>Sap/Drain</t>
+  </si>
+  <si>
+    <t>Berserk = ATT up, Speed Up, Defense Down</t>
+  </si>
+  <si>
+    <t>ATT, DEF, SPEED, MAG ATT, MAG DEF, LUCK</t>
+  </si>
+  <si>
+    <t>ATT Based MAG</t>
+  </si>
+  <si>
+    <t>DEF Based MAG</t>
+  </si>
+  <si>
+    <t>SPD Based MAG</t>
+  </si>
+  <si>
+    <t>LUCK based MAG</t>
+  </si>
+  <si>
+    <t>MAG ATT based MAG</t>
+  </si>
+  <si>
+    <t>MAG DEF based MAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spell Ideas: </t>
+  </si>
+  <si>
+    <t>Skill Buff</t>
+  </si>
+  <si>
+    <t>MAG ATT Buff</t>
+  </si>
+  <si>
+    <t>Luck Buff</t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t>Focus = MATT up, Speed up, Defense Down</t>
+  </si>
+  <si>
+    <t>Skill Buff = increases the proficiency points of each attribute of a skill temporarily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn </t>
+  </si>
+  <si>
+    <t>Electrocute</t>
+  </si>
+  <si>
+    <t>Freeze</t>
+  </si>
+  <si>
+    <t>Liquify</t>
+  </si>
+  <si>
+    <t>Harden</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn/Electrocute/Harden/Liquify/Freeze/Storm = Elemental Damage over time. </t>
+  </si>
+  <si>
+    <t>MP Poison</t>
+  </si>
+  <si>
+    <t>AP BUFF</t>
+  </si>
+  <si>
+    <t>Resist Ice</t>
+  </si>
+  <si>
+    <t>Resist Water</t>
+  </si>
+  <si>
+    <t>Resist Wind</t>
+  </si>
+  <si>
+    <t>Resist Lightning</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>Resist Fire</t>
+  </si>
+  <si>
+    <t>Resist Earth</t>
+  </si>
+  <si>
+    <t>Raises power by 25%</t>
+  </si>
+  <si>
+    <t>Summon Holy</t>
+  </si>
+  <si>
+    <t>Summon Fire</t>
+  </si>
+  <si>
+    <t>Summon Electric</t>
+  </si>
+  <si>
+    <t>Summon Earth</t>
+  </si>
+  <si>
+    <t>Summon Dark</t>
+  </si>
+  <si>
+    <t>Summon Water</t>
+  </si>
+  <si>
+    <t>Summon Ice</t>
+  </si>
+  <si>
+    <t>Summon Wind</t>
+  </si>
+  <si>
+    <t>A long pole with a blade or point on the end. The User gains a range advantage but sacrifices his ability to equip a shield.</t>
+  </si>
+  <si>
+    <t>but then it either always has to be square, or its going to end up being a fucked up polygon</t>
   </si>
 </sst>
 </file>
@@ -1427,7 +1523,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1512,11 +1608,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1564,6 +1697,41 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1880,479 +2048,603 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:M50"/>
+  <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="E2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G2" t="s">
+        <v>443</v>
+      </c>
+      <c r="H2" t="s">
+        <v>444</v>
+      </c>
+      <c r="I2" t="s">
+        <v>442</v>
+      </c>
+      <c r="K2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="37" t="s">
+        <v>465</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="37" t="s">
         <v>11</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="K5" t="s">
-        <v>445</v>
+      <c r="B5" s="30" t="s">
+        <v>469</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>474</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>475</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>75</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="M6" t="s">
-        <v>30</v>
+      <c r="B6" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="29" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>28</v>
+      <c r="B7" s="30" t="s">
+        <v>460</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>452</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>453</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>436</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>455</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>454</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>457</v>
+      </c>
+      <c r="J7" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>449</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="34" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="M9" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>462</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>459</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>466</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>467</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>425</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>447</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>448</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>432</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>1</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D12" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="32" t="s">
+        <v>445</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="E14" t="s">
+        <v>430</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="I14" s="32"/>
+      <c r="J14" s="41"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="9" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="1" t="s">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <f>(K25+(F25*1.3))</f>
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>468</v>
+      </c>
+      <c r="J25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K25">
         <v>10</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="1" t="s">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26">
+        <f>K26+(F26/4)</f>
+        <v>4</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26">
         <v>12</v>
       </c>
-      <c r="K10" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K11" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="F12" t="s">
-        <v>444</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>440</v>
-      </c>
-      <c r="K12" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="G26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C27">
+        <f>(K27+(F25*1.5)+(F26*1.5))*((75-F27)/75)+1</f>
+        <v>45.2</v>
+      </c>
+      <c r="E27" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21">
-        <f>(K21+(F21*1.3))</f>
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21">
-        <v>20</v>
-      </c>
-      <c r="G21" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21">
+      <c r="F27">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22">
-        <f>K22+(F22/4)</f>
-        <v>4</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22">
-        <v>12</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="G27" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>47</v>
       </c>
-      <c r="J22" t="s">
-        <v>43</v>
-      </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23">
-        <f>(K23+(F21*1.5)+(F22*1.5))*((75-F23)/75)+1</f>
-        <v>45.2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23">
-        <v>10</v>
-      </c>
-      <c r="G23" t="s">
-        <v>50</v>
-      </c>
-      <c r="J23" t="s">
-        <v>37</v>
-      </c>
-      <c r="K23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24">
-        <f>((K23+(F21*1.5)+(F22*1.5))/(((14+ F23) * 2)/50))</f>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28">
+        <f>((K27+(F25*1.5)+(F26*1.5))/(((14+ F27) * 2)/50))</f>
         <v>53.125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>157</v>
-      </c>
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25">
-        <f>(F21+ K23 +(F22*1.5)) - (F23*1.5)</f>
-        <v>26</v>
-      </c>
-      <c r="D25" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27">
-        <f>SUM(F21:F24)</f>
-        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>140</v>
+        <v>150</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <f>(F25+ K27 +(F26*1.5)) - (F27*1.5)</f>
+        <v>26</v>
+      </c>
+      <c r="D29" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>142</v>
+      <c r="E31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31">
+        <f>SUM(F25:F28)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>145</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C41" t="s">
-        <v>148</v>
-      </c>
-      <c r="D41" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" t="s">
-        <v>149</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>154</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="F44" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>155</v>
+      <c r="A47" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2360,8 +2652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,408 +2675,408 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
         <v>59</v>
-      </c>
-      <c r="B9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N21" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N22" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" t="s">
+        <v>178</v>
+      </c>
+      <c r="C24" t="s">
         <v>176</v>
       </c>
-      <c r="B24" t="s">
-        <v>185</v>
-      </c>
-      <c r="C24" t="s">
-        <v>183</v>
-      </c>
       <c r="E24" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="J24" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C25" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E25" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F25" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G25" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H25" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="J25" t="s">
-        <v>206</v>
+        <v>434</v>
       </c>
       <c r="N25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="O25" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P25" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="Q25" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="R25" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="S25" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B26" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E26" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="F26" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G26" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="H26" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="J26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="N26" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="O26" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="P26" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="Q26" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="R26" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="S26" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C27" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F27" t="s">
+        <v>201</v>
+      </c>
+      <c r="G27" t="s">
+        <v>202</v>
+      </c>
+      <c r="H27" t="s">
+        <v>203</v>
+      </c>
+      <c r="J27" t="s">
         <v>199</v>
       </c>
-      <c r="F27" t="s">
-        <v>209</v>
-      </c>
-      <c r="G27" t="s">
-        <v>210</v>
-      </c>
-      <c r="H27" t="s">
-        <v>211</v>
-      </c>
-      <c r="J27" t="s">
-        <v>207</v>
-      </c>
       <c r="N27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="O27" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="P27" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="Q27" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="R27" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="S27" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C28" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E28" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="F28" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G28" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="J28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N28" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="O28" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="P28" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
+        <v>184</v>
+      </c>
+      <c r="C29" t="s">
         <v>191</v>
-      </c>
-      <c r="C29" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C30" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C31" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E31" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="L31" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q31" t="s">
         <v>219</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C32" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E32" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="L32" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q32" t="s">
         <v>220</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L33" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q33" t="s">
         <v>221</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C34" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2808,326 +3100,326 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="G3" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="K3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="G4" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="I4" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="G5" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="L5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M5" t="s">
         <v>91</v>
       </c>
-      <c r="M5" t="s">
-        <v>96</v>
-      </c>
       <c r="Q5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="S5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="G6" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="L6" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" t="s">
         <v>92</v>
       </c>
-      <c r="M6" t="s">
-        <v>97</v>
-      </c>
       <c r="Q6" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="S6" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="G7" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="L7" t="s">
+        <v>88</v>
+      </c>
+      <c r="M7" t="s">
         <v>93</v>
       </c>
-      <c r="M7" t="s">
-        <v>98</v>
-      </c>
       <c r="Q7" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="S7" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="G8" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="L8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="M8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="Q8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="S8" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G9" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="L9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="M9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="Q9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="S9" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L10" t="s">
+        <v>94</v>
+      </c>
+      <c r="M10" t="s">
         <v>99</v>
       </c>
-      <c r="M10" t="s">
-        <v>104</v>
-      </c>
       <c r="Q10" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="S10" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="Q11" t="s">
+        <v>160</v>
+      </c>
+      <c r="S11" t="s">
         <v>167</v>
-      </c>
-      <c r="S11" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="L12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="M12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="L13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="M13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L14" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="M14" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L15" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L16" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M16" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B18" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H19" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H20" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C26" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C27" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3140,7 +3432,7 @@
   <dimension ref="A1:E258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3151,26 +3443,26 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E3" t="s">
         <v>244</v>
-      </c>
-      <c r="E3" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -6496,8 +6788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6517,646 +6809,646 @@
   <sheetData>
     <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B4" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="C4" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D4" t="s">
-        <v>317</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>328</v>
+        <v>309</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>320</v>
       </c>
       <c r="F4" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="G4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E5" s="30"/>
+      <c r="E5" s="43"/>
       <c r="G5" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="30"/>
+      <c r="E6" s="43"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B7" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C7" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D7" t="s">
-        <v>317</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>329</v>
+        <v>309</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>321</v>
       </c>
       <c r="F7" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="G7" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="M7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E8" s="29"/>
+      <c r="E8" s="42"/>
       <c r="G8" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E9" s="29"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B10" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="C10" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D10" t="s">
-        <v>317</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>330</v>
+        <v>309</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>322</v>
       </c>
       <c r="F10" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="G10" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M10" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E11" s="29"/>
+      <c r="E11" s="42"/>
       <c r="F11" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="G11" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E12" s="29"/>
+      <c r="E12" s="42"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C13" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D13" t="s">
-        <v>317</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>331</v>
+        <v>309</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>323</v>
       </c>
       <c r="F13" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="G13" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="M13" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E14" s="29"/>
+      <c r="E14" s="42"/>
       <c r="G14" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E15" s="29"/>
+      <c r="E15" s="42"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C16" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D16" t="s">
-        <v>317</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>334</v>
+        <v>309</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>326</v>
       </c>
       <c r="F16" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="G16" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="M16" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E17" s="31"/>
+      <c r="E17" s="44"/>
       <c r="G17" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E18" s="31"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>335</v>
+        <v>309</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>327</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="G19" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M19" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="29"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="3"/>
       <c r="G20" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E21" s="29"/>
+      <c r="E21" s="42"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B22" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C22" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D22" t="s">
-        <v>289</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>336</v>
+        <v>281</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>328</v>
       </c>
       <c r="F22" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="G22" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M22" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E23" s="29"/>
+      <c r="E23" s="42"/>
       <c r="G23" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E24" s="29"/>
+      <c r="E24" s="42"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B25" t="s">
+        <v>275</v>
+      </c>
+      <c r="C25" t="s">
+        <v>310</v>
+      </c>
+      <c r="D25" t="s">
+        <v>281</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="F25" t="s">
+        <v>330</v>
+      </c>
+      <c r="G25" t="s">
+        <v>266</v>
+      </c>
+      <c r="M25" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E26" s="42"/>
+      <c r="F26" t="s">
+        <v>332</v>
+      </c>
+      <c r="G26" t="s">
         <v>283</v>
       </c>
-      <c r="C25" t="s">
-        <v>318</v>
-      </c>
-      <c r="D25" t="s">
-        <v>289</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>339</v>
-      </c>
-      <c r="F25" t="s">
-        <v>338</v>
-      </c>
-      <c r="G25" t="s">
-        <v>274</v>
-      </c>
-      <c r="M25" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E26" s="29"/>
-      <c r="F26" t="s">
-        <v>340</v>
-      </c>
-      <c r="G26" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E27" s="29"/>
+      <c r="E27" s="42"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B28" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C28" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D28" t="s">
-        <v>322</v>
-      </c>
-      <c r="E28" s="31" t="s">
-        <v>341</v>
+        <v>314</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>333</v>
       </c>
       <c r="F28" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G28" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M28" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E29" s="31"/>
+      <c r="E29" s="44"/>
       <c r="F29" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="G29" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E30" s="31"/>
+      <c r="E30" s="44"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B31" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C31" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D31" t="s">
-        <v>317</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>344</v>
+        <v>309</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>336</v>
       </c>
       <c r="F31" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G31" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M31" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E32" s="31"/>
+      <c r="E32" s="44"/>
       <c r="G32" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E33" s="31"/>
+      <c r="E33" s="44"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B34" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C34" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D34" t="s">
-        <v>317</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>345</v>
+        <v>309</v>
+      </c>
+      <c r="E34" s="44" t="s">
+        <v>337</v>
       </c>
       <c r="F34" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="G34" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M34" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E35" s="31"/>
+      <c r="E35" s="44"/>
       <c r="G35" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E36" s="31"/>
+      <c r="E36" s="44"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B37" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C37" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D37" t="s">
-        <v>317</v>
-      </c>
-      <c r="E37" s="31" t="s">
-        <v>347</v>
+        <v>309</v>
+      </c>
+      <c r="E37" s="44" t="s">
+        <v>339</v>
       </c>
       <c r="F37" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G37" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M37" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E38" s="31"/>
+      <c r="E38" s="44"/>
       <c r="G38" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E39" s="31"/>
+      <c r="E39" s="44"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B40" t="s">
+        <v>276</v>
+      </c>
+      <c r="C40" t="s">
+        <v>310</v>
+      </c>
+      <c r="D40" t="s">
+        <v>315</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>340</v>
+      </c>
+      <c r="F40" t="s">
+        <v>330</v>
+      </c>
+      <c r="G40" t="s">
+        <v>266</v>
+      </c>
+      <c r="M40" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E41" s="42"/>
+      <c r="F41" t="s">
+        <v>324</v>
+      </c>
+      <c r="G41" t="s">
         <v>284</v>
       </c>
-      <c r="C40" t="s">
-        <v>318</v>
-      </c>
-      <c r="D40" t="s">
-        <v>323</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>348</v>
-      </c>
-      <c r="F40" t="s">
-        <v>338</v>
-      </c>
-      <c r="G40" t="s">
-        <v>274</v>
-      </c>
-      <c r="M40" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E41" s="29"/>
-      <c r="F41" t="s">
-        <v>332</v>
-      </c>
-      <c r="G41" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E42" s="29"/>
+      <c r="E42" s="42"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B43" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C43" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D43" t="s">
-        <v>323</v>
-      </c>
-      <c r="E43" s="29" t="s">
-        <v>349</v>
+        <v>315</v>
+      </c>
+      <c r="E43" s="42" t="s">
+        <v>341</v>
       </c>
       <c r="F43" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="G43" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M43" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E44" s="29"/>
+      <c r="E44" s="42"/>
       <c r="F44" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G44" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E45" s="29"/>
+      <c r="E45" s="42"/>
       <c r="F45" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B46" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C46" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D46" t="s">
-        <v>322</v>
-      </c>
-      <c r="E46" s="29" t="s">
-        <v>350</v>
+        <v>314</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>477</v>
       </c>
       <c r="F46" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="G46" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M46" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E47" s="29"/>
+      <c r="E47" s="42"/>
       <c r="F47" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="G47" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E48" s="29"/>
+      <c r="E48" s="42"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>301</v>
+      </c>
+      <c r="B49" t="s">
+        <v>313</v>
+      </c>
+      <c r="C49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D49" t="s">
         <v>309</v>
       </c>
-      <c r="B49" t="s">
-        <v>321</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="E49" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="F49" t="s">
         <v>324</v>
       </c>
-      <c r="D49" t="s">
-        <v>317</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>352</v>
-      </c>
-      <c r="F49" t="s">
-        <v>332</v>
-      </c>
       <c r="G49" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M49" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E50" s="31"/>
+      <c r="E50" s="44"/>
       <c r="F50" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G50" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E51" s="31"/>
+      <c r="E51" s="44"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -7186,8 +7478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7206,41 +7498,41 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="32" t="s">
-        <v>262</v>
-      </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="33"/>
+      <c r="C8" s="45" t="s">
+        <v>253</v>
+      </c>
+      <c r="D8" s="46"/>
+      <c r="E8" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="F8" s="46"/>
+      <c r="G8" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="H8" s="46"/>
+      <c r="I8" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="46"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C9" s="10">
         <v>1</v>
@@ -7271,7 +7563,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C10" s="10">
         <v>1</v>
@@ -7302,7 +7594,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C11" s="10">
         <v>5</v>
@@ -7333,7 +7625,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C12" s="10">
         <v>1</v>
@@ -7372,7 +7664,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
@@ -7385,7 +7677,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
@@ -7408,7 +7700,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C17" s="10">
         <f>C11 + (1+C9*C10)</f>
@@ -7433,7 +7725,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C18" s="10">
         <f>(C11*1.25)+(1+C9*C10)</f>
@@ -7468,7 +7760,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C20" s="10">
         <f>C17 - (C17*(C12/128))</f>
@@ -7513,7 +7805,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C23" s="10">
         <f>((C9+C10)*C11-C12)</f>
@@ -7538,7 +7830,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C24" s="10">
         <f>C23-(C23*(C12/128))</f>
@@ -7573,32 +7865,32 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="13" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -7700,300 +7992,300 @@
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C31" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I31" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C34" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="I34" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="I37" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C40" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I40" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C43" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="I43" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C46" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I46" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C47" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B49" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C49" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I49" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B52" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C52" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I52" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B55" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C55" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I55" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="J55" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C58" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I58" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="J58" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C61" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I61" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="J61" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C64" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I64" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="J64" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B67" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C67" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I67" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B70" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C70" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I70" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B73" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="C73" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I73" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B76" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="C76" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I76" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -8012,7 +8304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A85"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
@@ -8020,387 +8312,387 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>